<commit_message>
Fixed test w.r.t personnel header change
</commit_message>
<xml_diff>
--- a/t/Personnel.xlsx
+++ b/t/Personnel.xlsx
@@ -28,9 +28,6 @@
     <t>EM</t>
   </si>
   <si>
-    <t>Dienstverlening</t>
-  </si>
-  <si>
     <t>Onderzoek</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Danny.Bhoy@ua.ac.be</t>
+  </si>
+  <si>
+    <t>Dienst-verlening</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -637,7 +637,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -655,50 +655,50 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="F7" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" ref="C9:C16" si="0">CONCATENATE(A9," ",B9)</f>
         <v>GI Joe</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
@@ -715,17 +715,17 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Dumbhead Dirk</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -742,17 +742,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Sporgese Ellen</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -769,17 +769,17 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Ketten Dick</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -796,17 +796,17 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MacAllen Bob</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>1</v>
@@ -823,17 +823,17 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Frog Frank</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -850,17 +850,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Bindozer Walter</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -877,17 +877,17 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Bhoy Danny</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>

</xml_diff>